<commit_message>
assuring the standard measures are always available
</commit_message>
<xml_diff>
--- a/doc/examples/forecasting/forecast-netting.xlsx
+++ b/doc/examples/forecasting/forecast-netting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\enterprise\doc\user-guide\examples\forecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\jdetaeye\workspace\frepple-community\doc\examples\forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8380866A-D83E-41DC-BDE4-BC7388F81829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CFF6C6-1653-4BC1-8070-7D526AC46230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="20000" windowHeight="12100" tabRatio="835" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,74 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{92E2512E-67F5-4CB6-9DAB-8772FF14B834}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Accepted values are: aggregate, local, computed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{CECFD419-4DEA-4129-8B9A-9BF912CF30B5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Accepted values are: edit, view, hide</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{43888847-E50C-49C9-B1C3-0003CED0A3ED}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Accepted values are: edit, view, hide</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{3E078421-A260-4EDE-B0EB-B30AC9A3FAB8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Accepted values are: number, currency</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -301,15 +367,9 @@
     <t>Value</t>
   </si>
   <si>
-    <t>allowsplits</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
-    <t>Controls whether a sales order or forecast can be split across multiple manufacturing orders during planning. Default: true</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
@@ -817,9 +877,6 @@
     <t>Initially Hidden</t>
   </si>
   <si>
-    <t>Formatter</t>
-  </si>
-  <si>
     <t>Default Value</t>
   </si>
   <si>
@@ -863,6 +920,135 @@
   </si>
   <si>
     <t>if(cost != 0, forecasttotal:= newvalue /cost, forecasttotalvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>forecastbaselinevalue</t>
+  </si>
+  <si>
+    <t>forecast baseline value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, forecastbaselinevalue, forecastbaseline * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, forecastbaseline := newvalue /cost, forecastbaselinevalue := newvalue)</t>
+  </si>
+  <si>
+    <t>forecastconsumedvalue</t>
+  </si>
+  <si>
+    <t>forecast consumed value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, forecastconsumedvalue, forecastconsumed * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, forecastconsumed := newvalue / cost, forecastconsumedvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>forecastnetvalue</t>
+  </si>
+  <si>
+    <t>forecast net value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, forecastnetvalue, forecastnet * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, forecastnet := newvalue /cost, forecastnetvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>forecastoverridevalue</t>
+  </si>
+  <si>
+    <t>forecast override value</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>if(cost == 0, forecastoverridevalue, if(forecastoverride == -1, -1, forecastoverride * cost))</t>
+  </si>
+  <si>
+    <t>if(cost != 0, forecastoverride := if(newvalue == -1, -1, newvalue / cost), forecastoverridevalue := newvalue)</t>
+  </si>
+  <si>
+    <t>forecastplannedvalue</t>
+  </si>
+  <si>
+    <t>planned forecast value</t>
+  </si>
+  <si>
+    <t>hide</t>
+  </si>
+  <si>
+    <t>if(cost == 0, forecastplannedvalue, forecastplanned * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, forecastplanned := newvalue /cost, forecastplannedvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>nodata</t>
+  </si>
+  <si>
+    <t>no data</t>
+  </si>
+  <si>
+    <t>Indicates gaps in the sales history</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>ordersadjustmentvalue</t>
+  </si>
+  <si>
+    <t>orders adjustment value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, ordersadjustmentvalue, ordersadjustment * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, ordersadjustment := newvalue /cost, ordersadjustmentvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>ordersopenvalue</t>
+  </si>
+  <si>
+    <t>orders open value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, ordersopenvalue, ordersopen * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, ordersopen := newvalue /cost, ordersopenvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>ordersplannedvalue</t>
+  </si>
+  <si>
+    <t>planned orders value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, ordersplannedvalue, ordersplanned * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, ordersplanned := newvalue /cost, ordersplannedvalue := newvalue)</t>
+  </si>
+  <si>
+    <t>orderstotalvalue</t>
+  </si>
+  <si>
+    <t>orders total value</t>
+  </si>
+  <si>
+    <t>if(cost == 0, orderstotalvalue, orderstotal * cost)</t>
+  </si>
+  <si>
+    <t>if(cost != 0, orderstotal := newvalue /cost, orderstotalvalue := newvalue)</t>
   </si>
 </sst>
 </file>
@@ -872,7 +1058,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -917,13 +1103,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1235,12 +1417,12 @@
       <selection activeCell="I1" sqref="I1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1318,7 +1500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1344,7 +1526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1370,7 +1552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1422,7 +1604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1474,7 +1656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1500,7 +1682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1526,7 +1708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1552,7 +1734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1578,7 +1760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1604,7 +1786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1630,7 +1812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1656,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1682,7 +1864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1708,7 +1890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1734,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1760,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1786,7 +1968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1812,7 +1994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1838,7 +2020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1864,7 +2046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1890,7 +2072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1916,7 +2098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1942,7 +2124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1968,7 +2150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1994,7 +2176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2020,7 +2202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -2046,7 +2228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2072,7 +2254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2098,7 +2280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2150,7 +2332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2202,7 +2384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2228,7 +2410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2254,7 +2436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2280,7 +2462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2306,7 +2488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2332,7 +2514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -2358,7 +2540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -2384,7 +2566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -2410,7 +2592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -2436,7 +2618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -2462,7 +2644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -2488,7 +2670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -2514,7 +2696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -2540,7 +2722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -2566,7 +2748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -2592,7 +2774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -2632,13 +2814,13 @@
       <selection activeCell="C1" sqref="C1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2646,12 +2828,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2659,7 +2841,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -2681,14 +2863,14 @@
       <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2707,12 +2889,12 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2720,12 +2902,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2733,7 +2915,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2755,20 +2937,20 @@
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -2823,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -2849,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -2875,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -2901,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -2927,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -2967,14 +3149,14 @@
       <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -2993,9 +3175,9 @@
       <selection activeCell="G1" sqref="G1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3015,7 +3197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -3040,19 +3222,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="182.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="182.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3063,899 +3245,1213 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" t="s">
-        <v>112</v>
       </c>
       <c r="C10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" t="s">
-        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>135</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" t="s">
-        <v>150</v>
       </c>
       <c r="C24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>154</v>
-      </c>
-      <c r="B26" t="s">
-        <v>155</v>
       </c>
       <c r="C26" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>157</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>162</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="s">
         <v>164</v>
       </c>
-      <c r="B30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>165</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>167</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>173</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
       <c r="C38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" t="s">
         <v>185</v>
       </c>
-      <c r="B40" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>186</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>188</v>
       </c>
-      <c r="B42" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>189</v>
       </c>
-      <c r="B43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" t="s">
         <v>190</v>
       </c>
-      <c r="B44" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>191</v>
       </c>
       <c r="B45" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C47" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B48" t="s">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>202</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>203</v>
       </c>
       <c r="C49" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>209</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>211</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>213</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="C54" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C55" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B56" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C56" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B57" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>224</v>
       </c>
       <c r="B58" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="C58" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B59" t="s">
-        <v>227</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>229</v>
       </c>
       <c r="B60" t="s">
-        <v>144</v>
+        <v>230</v>
       </c>
       <c r="C60" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>231</v>
-      </c>
-      <c r="B61" t="s">
         <v>232</v>
       </c>
       <c r="C61" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>234</v>
       </c>
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
       <c r="C62" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>236</v>
       </c>
       <c r="B63" t="s">
-        <v>144</v>
+        <v>237</v>
       </c>
       <c r="C63" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B64" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
       <c r="C64" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>241</v>
       </c>
       <c r="B65" t="s">
-        <v>197</v>
+        <v>87</v>
       </c>
       <c r="C65" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>243</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>244</v>
       </c>
       <c r="C66" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B67" t="s">
-        <v>246</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>248</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>250</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>252</v>
-      </c>
-      <c r="B70" t="s">
-        <v>88</v>
-      </c>
-      <c r="C70" t="s">
-        <v>253</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:C1048575" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE69CCF3-41BA-4C72-BA27-7852D0B767C5}">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE69CCF3-41BA-4C72-BA27-7852D0B767C5}">
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="77.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="93" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="K1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>275</v>
+      </c>
+      <c r="L2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>279</v>
+      </c>
+      <c r="L3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F4" t="s">
+        <v>265</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>288</v>
+      </c>
+      <c r="L5" t="s">
+        <v>289</v>
+      </c>
+      <c r="M5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>293</v>
+      </c>
+      <c r="L6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>261</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="B7" t="s">
         <v>262</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="C7" t="s">
         <v>263</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="3" t="s">
+      <c r="D7" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E7" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F7" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
         <v>266</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>267</v>
       </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>268</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G2" s="3" t="b">
+      <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" t="s">
+        <v>265</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8">
         <v>0</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3">
+      <c r="K8" t="s">
+        <v>270</v>
+      </c>
+      <c r="L8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" t="s">
+        <v>297</v>
+      </c>
+      <c r="D9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>266</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G3" s="3" t="b">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D10" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" t="s">
+        <v>292</v>
+      </c>
+      <c r="G10" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3">
+      <c r="H10" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10">
         <v>0</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="6"/>
+      <c r="K10" t="s">
+        <v>301</v>
+      </c>
+      <c r="L10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" t="s">
+        <v>265</v>
+      </c>
+      <c r="F11" t="s">
+        <v>265</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>305</v>
+      </c>
+      <c r="L11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+      <c r="D12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F12" t="s">
+        <v>265</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>309</v>
+      </c>
+      <c r="L12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F13" t="s">
+        <v>265</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>313</v>
+      </c>
+      <c r="L13" t="s">
+        <v>314</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>